<commit_message>
création code partie graph
modification du MCD et du MLD
modification maquette
modification journal de travail
création du code la partie graphique
</commit_message>
<xml_diff>
--- a/journal de travail/Journal_travail.xlsx
+++ b/journal de travail/Journal_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>scénarii fini, use case fini et maquette fini</t>
+  </si>
+  <si>
+    <t>modication MCD et MLD</t>
+  </si>
+  <si>
+    <t>45min</t>
+  </si>
+  <si>
+    <t>début du code partie graphique</t>
   </si>
 </sst>
 </file>
@@ -605,7 +614,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,19 +716,31 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="14"/>
+      <c r="A8" s="4">
+        <v>43133</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="11"/>
+      <c r="D8" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="14"/>
+      <c r="A9" s="4">
+        <v>43133</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
       <c r="G9" s="5"/>

</xml_diff>

<commit_message>
début du code C#
</commit_message>
<xml_diff>
--- a/journal de travail/Journal_travail.xlsx
+++ b/journal de travail/Journal_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>début du code partie graphique</t>
+  </si>
+  <si>
+    <t>modification MCD et MLD et fini la partie graphique, début code login</t>
   </si>
 </sst>
 </file>
@@ -295,15 +298,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,6 +323,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -614,7 +617,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,52 +635,52 @@
         <v>5</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="19"/>
+      <c r="F1" s="16"/>
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43129</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="27"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43132</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
@@ -746,10 +749,16 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="14"/>
+      <c r="A10" s="4">
+        <v>43136</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>16</v>
+      </c>
       <c r="C10" s="15"/>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
       <c r="G10" s="5"/>
@@ -918,51 +927,51 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
-      <c r="B29" s="16"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="15"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="16"/>
+      <c r="E29" s="25"/>
       <c r="F29" s="15"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="16"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="15"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="16"/>
+      <c r="E30" s="25"/>
       <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="16"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="15"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="16"/>
+      <c r="E31" s="25"/>
       <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="16"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="15"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="25"/>
       <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="16"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="15"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="25"/>
       <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="16"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="15"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="16"/>
+      <c r="E34" s="25"/>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,294 +979,203 @@
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="16"/>
+      <c r="E35" s="25"/>
       <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="16"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="15"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="16"/>
+      <c r="E36" s="25"/>
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="27"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="18"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="16"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="16"/>
-      <c r="C41" s="16"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="16"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="16"/>
-      <c r="C47" s="16"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="16"/>
-      <c r="C49" s="16"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="16"/>
-      <c r="C51" s="16"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="16"/>
-      <c r="C53" s="16"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="16"/>
-      <c r="C54" s="16"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="16"/>
-      <c r="C55" s="16"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="25"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="25"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="25"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="16"/>
-      <c r="C60" s="16"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="25"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="16"/>
-      <c r="C61" s="16"/>
+      <c r="B61" s="25"/>
+      <c r="C61" s="25"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="16"/>
-      <c r="C62" s="16"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="25"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="16"/>
-      <c r="C63" s="16"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="25"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="25"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="25"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="25"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="25"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
+      <c r="B73" s="25"/>
+      <c r="C73" s="25"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="25"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
+      <c r="B75" s="25"/>
+      <c r="C75" s="25"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="25"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
+      <c r="B81" s="25"/>
+      <c r="C81" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="115">
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
@@ -1282,6 +1200,97 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fin de la classe cryptage
</commit_message>
<xml_diff>
--- a/journal de travail/Journal_travail.xlsx
+++ b/journal de travail/Journal_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>modification MCD et MLD et fini la partie graphique, début code login</t>
+  </si>
+  <si>
+    <t>absent du au décès de ma grand-maman</t>
+  </si>
+  <si>
+    <t>recherche d'une methode de cryptage du mot de passe</t>
+  </si>
+  <si>
+    <t>création de la classe cryptage</t>
   </si>
 </sst>
 </file>
@@ -617,7 +626,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,28 +773,46 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="14"/>
+      <c r="A11" s="4">
+        <v>43137</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="4">
+        <v>43139</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="14"/>
+      <c r="A13" s="4">
+        <v>43139</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
       <c r="G13" s="5"/>

</xml_diff>

<commit_message>
creation des classe Produit, Location, Loueur
</commit_message>
<xml_diff>
--- a/journal de travail/Journal_travail.xlsx
+++ b/journal de travail/Journal_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>modification MLD</t>
+  </si>
+  <si>
+    <t>code classe Produit, Loueur, Location, et connection bd</t>
   </si>
 </sst>
 </file>
@@ -310,6 +313,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -335,15 +347,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -629,7 +632,7 @@
   <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:C14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,52 +650,52 @@
         <v>5</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="16"/>
+      <c r="F1" s="19"/>
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="23"/>
+      <c r="F3" s="26"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>43129</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="24"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="27"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43132</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="11" t="s">
         <v>7</v>
       </c>
@@ -836,19 +839,31 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="14"/>
+      <c r="A15" s="4">
+        <v>43140</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="C15" s="15"/>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="14"/>
+      <c r="A16" s="4">
+        <v>43143</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>21</v>
+      </c>
       <c r="C16" s="15"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
       <c r="G16" s="5"/>
@@ -963,51 +978,51 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
-      <c r="B29" s="25"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="15"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="25"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="15"/>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="25"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="15"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="25"/>
+      <c r="E30" s="16"/>
       <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="25"/>
+      <c r="B31" s="16"/>
       <c r="C31" s="15"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="25"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
-      <c r="B32" s="25"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="15"/>
       <c r="D32" s="11"/>
-      <c r="E32" s="25"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="25"/>
+      <c r="B33" s="16"/>
       <c r="C33" s="15"/>
       <c r="D33" s="11"/>
-      <c r="E33" s="25"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="25"/>
+      <c r="B34" s="16"/>
       <c r="C34" s="15"/>
       <c r="D34" s="11"/>
-      <c r="E34" s="25"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,203 +1030,294 @@
       <c r="B35" s="14"/>
       <c r="C35" s="15"/>
       <c r="D35" s="11"/>
-      <c r="E35" s="25"/>
+      <c r="E35" s="16"/>
       <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="25"/>
+      <c r="B36" s="16"/>
       <c r="C36" s="15"/>
       <c r="D36" s="11"/>
-      <c r="E36" s="25"/>
+      <c r="E36" s="16"/>
       <c r="F36" s="15"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="9"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="27"/>
+      <c r="B37" s="17"/>
+      <c r="C37" s="18"/>
       <c r="D37" s="13"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="16"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="25"/>
-      <c r="C55" s="25"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="25"/>
-      <c r="C56" s="25"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="25"/>
-      <c r="C57" s="25"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="25"/>
-      <c r="C58" s="25"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="25"/>
-      <c r="C59" s="25"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="25"/>
-      <c r="C60" s="25"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="25"/>
-      <c r="C64" s="25"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="25"/>
-      <c r="C65" s="25"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
+      <c r="B67" s="16"/>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="25"/>
-      <c r="C69" s="25"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="25"/>
-      <c r="C70" s="25"/>
+      <c r="B70" s="16"/>
+      <c r="C70" s="16"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
+      <c r="B71" s="16"/>
+      <c r="C71" s="16"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="25"/>
-      <c r="C72" s="25"/>
+      <c r="B72" s="16"/>
+      <c r="C72" s="16"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="25"/>
-      <c r="C73" s="25"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="25"/>
-      <c r="C75" s="25"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="16"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
+      <c r="B78" s="16"/>
+      <c r="C78" s="16"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
+      <c r="B80" s="16"/>
+      <c r="C80" s="16"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
+      <c r="B81" s="16"/>
+      <c r="C81" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="115">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
@@ -1236,97 +1342,6 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
remise au propre et test
</commit_message>
<xml_diff>
--- a/journal de travail/Journal_travail.xlsx
+++ b/journal de travail/Journal_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>débug</t>
+  </si>
+  <si>
+    <t>remise au propre des classes XML et Config et Classe sur Astah</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -411,65 +417,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,1016 +779,923 @@
         <v>4</v>
       </c>
       <c r="D1" s="1"/>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="27"/>
+      <c r="F1" s="18"/>
       <c r="G1" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="32"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43129</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="30"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="9">
         <v>90</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="33"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="26"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>43132</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="6">
         <v>90</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>43132</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="15"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="6">
         <v>135</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>43132</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="17"/>
       <c r="D7" s="6">
         <v>90</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>43133</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="6">
         <v>45</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>43133</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="6">
         <v>45</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>43136</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="17"/>
       <c r="D10" s="6">
         <v>90</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>43137</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="6">
         <v>90</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>43139</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="17"/>
       <c r="D12" s="6">
         <v>90</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>43139</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="6">
         <v>135</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>43139</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="15"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="6">
         <v>90</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>43140</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="6">
         <v>90</v>
       </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>43143</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="6">
         <v>90</v>
       </c>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>43144</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="6">
         <v>90</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>43146</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="6">
         <v>315</v>
       </c>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>43147</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="17"/>
       <c r="D19" s="6">
         <v>90</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>43157</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="6">
         <v>90</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>43158</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="6">
         <v>90</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>43160</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="17"/>
       <c r="D22" s="6">
         <v>315</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>43161</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="17"/>
       <c r="D23" s="6">
         <v>90</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>43164</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="17"/>
       <c r="D24" s="6">
         <v>90</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>43165</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="6">
         <v>55</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="24"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>43165</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="6">
         <v>65</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>43167</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="6">
         <v>45</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>43167</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="24"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="6">
         <v>10</v>
       </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>43167</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="6">
         <v>30</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="15"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="17"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>43167</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="6">
         <v>135</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="15"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>43167</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="6">
         <v>45</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="15"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>43167</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="6">
         <v>20</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="15"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>43167</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="15"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="6">
         <v>25</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="15"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>43168</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="15"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="6">
         <v>45</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="15"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>43168</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="15"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="6">
         <v>45</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="15"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>43171</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="15"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="6">
         <v>90</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F36" s="15"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12">
         <v>43172</v>
       </c>
-      <c r="B37" s="21" t="s">
+      <c r="B37" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="29"/>
       <c r="D37" s="10">
         <v>90</v>
       </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="26"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="12">
         <v>43174</v>
       </c>
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="15"/>
       <c r="D38" s="13">
         <v>10</v>
       </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="12">
         <v>43174</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="17"/>
+      <c r="C39" s="14"/>
       <c r="D39" s="13">
         <v>10</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="12">
         <v>43174</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C40" s="17"/>
+      <c r="C40" s="14"/>
       <c r="D40" s="13">
         <v>70</v>
       </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="12">
         <v>43174</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="17"/>
+      <c r="C41" s="14"/>
       <c r="D41" s="13">
         <v>90</v>
       </c>
-      <c r="E41" s="17" t="s">
+      <c r="E41" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="17"/>
+      <c r="F41" s="14"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="12">
         <v>43174</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="17"/>
+      <c r="C42" s="14"/>
       <c r="D42" s="13">
         <v>20</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="17"/>
+      <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="12">
         <v>43174</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="14"/>
       <c r="D43" s="13">
         <v>70</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="17"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="12">
         <v>43175</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="17"/>
+      <c r="C44" s="14"/>
       <c r="D44" s="13">
         <v>20</v>
       </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12">
         <v>43175</v>
       </c>
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="18"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="13">
         <v>70</v>
       </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="12">
         <v>43178</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="17"/>
+      <c r="C46" s="14"/>
       <c r="D46" s="13">
         <v>90</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="12">
         <v>43179</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="17"/>
+      <c r="C47" s="14"/>
       <c r="D47" s="13">
         <v>45</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="12">
         <v>43179</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="17"/>
+      <c r="C48" s="14"/>
       <c r="D48" s="13">
         <v>20</v>
       </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
         <v>43179</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="17"/>
+      <c r="C49" s="14"/>
       <c r="D49" s="13">
         <v>25</v>
       </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
+      <c r="A50" s="12">
+        <v>43181</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="13">
+        <v>65</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
+      <c r="A51" s="12">
+        <v>43181</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="13">
+        <v>35</v>
+      </c>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="17"/>
-      <c r="F52" s="17"/>
+      <c r="A52" s="12">
+        <v>43181</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="13">
+        <v>125</v>
+      </c>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="17"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17"/>
+      <c r="A53" s="12">
+        <v>43181</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="13">
+        <v>90</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
       <c r="D54" s="13"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="17"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
       <c r="D55" s="13"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="12"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
       <c r="D56" s="13"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
       <c r="D57" s="13"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
       <c r="D58" s="13"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="17"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
       <c r="D59" s="13"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="12"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
       <c r="D60" s="13"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="12"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="17"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
       <c r="D61" s="13"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
       <c r="D62" s="13"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
       <c r="D63" s="13"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="16"/>
-      <c r="C64" s="16"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="33"/>
       <c r="D64">
         <f>SUM(D4:D63)</f>
-        <v>3580</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
+      <c r="B65" s="33"/>
+      <c r="C65" s="33"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="16"/>
-      <c r="C66" s="16"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="16"/>
-      <c r="C67" s="16"/>
+      <c r="B67" s="33"/>
+      <c r="C67" s="33"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
+      <c r="B68" s="33"/>
+      <c r="C68" s="33"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="16"/>
-      <c r="C69" s="16"/>
+      <c r="B69" s="33"/>
+      <c r="C69" s="33"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="16"/>
-      <c r="C70" s="16"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="33"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
+      <c r="B71" s="33"/>
+      <c r="C71" s="33"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="16"/>
-      <c r="C72" s="16"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="33"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="16"/>
-      <c r="C73" s="16"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="33"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="16"/>
-      <c r="C75" s="16"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="33"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="16"/>
-      <c r="C76" s="16"/>
+      <c r="B76" s="33"/>
+      <c r="C76" s="33"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="16"/>
-      <c r="C77" s="16"/>
+      <c r="B77" s="33"/>
+      <c r="C77" s="33"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="16"/>
-      <c r="C78" s="16"/>
+      <c r="B78" s="33"/>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="16"/>
-      <c r="C79" s="16"/>
+      <c r="B79" s="33"/>
+      <c r="C79" s="33"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="16"/>
-      <c r="C80" s="16"/>
+      <c r="B80" s="33"/>
+      <c r="C80" s="33"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="16"/>
-      <c r="C81" s="16"/>
+      <c r="B81" s="33"/>
+      <c r="C81" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="E16:F16"/>
@@ -1807,6 +1720,123 @@
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>